<commit_message>
Import to multiple tables and course addition
</commit_message>
<xml_diff>
--- a/public/uploads/class_list_sample.xlsx
+++ b/public/uploads/class_list_sample.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Dropbox\PC\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,9 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>student_name</t>
-  </si>
-  <si>
     <t>matric_no</t>
   </si>
   <si>
@@ -42,6 +39,9 @@
   </si>
   <si>
     <t>19/3423</t>
+  </si>
+  <si>
+    <t>name</t>
   </si>
 </sst>
 </file>
@@ -370,9 +370,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -382,26 +380,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>